<commit_message>
boruvka step 1 has been tested
</commit_message>
<xml_diff>
--- a/excel/karger_burma14.xlsx
+++ b/excel/karger_burma14.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dokumenty\studia\praca_dyplomowa\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dokumenty\studia\praca_dyplomowa\git_magisterka\magisterka\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7F214E-5125-4E55-ACD7-2FCD768AA472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7B161C-EEDB-419B-8729-D1EE83C96235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{7A6D875E-0F67-4653-8D10-21F433F1A622}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7A6D875E-0F67-4653-8D10-21F433F1A622}"/>
   </bookViews>
   <sheets>
     <sheet name="Boruvka step 1" sheetId="1" r:id="rId1"/>
@@ -232,10 +232,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>528687</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>173624</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -258,8 +258,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="12252960"/>
-          <a:ext cx="3363327" cy="2514600"/>
+          <a:off x="0" y="12763500"/>
+          <a:ext cx="5570220" cy="4364624"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -619,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB8272D6-92E0-46DF-A61E-1D1AF8F3CB02}">
   <dimension ref="A1:X67"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="R43" sqref="R43"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="N85" sqref="N85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3070,18 +3070,50 @@
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="N54:N55"/>
-    <mergeCell ref="N56:N57"/>
-    <mergeCell ref="N58:N59"/>
-    <mergeCell ref="I54:I55"/>
-    <mergeCell ref="I56:I57"/>
-    <mergeCell ref="I58:I59"/>
-    <mergeCell ref="I60:I61"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="S50:S51"/>
+    <mergeCell ref="S52:S53"/>
+    <mergeCell ref="S54:S55"/>
+    <mergeCell ref="S56:S57"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="I36:I37"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="I40:I41"/>
+    <mergeCell ref="I42:I43"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="S36:S37"/>
+    <mergeCell ref="S38:S39"/>
+    <mergeCell ref="N32:N33"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="N26:N27"/>
+    <mergeCell ref="N28:N29"/>
+    <mergeCell ref="N30:N31"/>
+    <mergeCell ref="S22:S23"/>
+    <mergeCell ref="S24:S25"/>
+    <mergeCell ref="S26:S27"/>
+    <mergeCell ref="S28:S29"/>
+    <mergeCell ref="S30:S31"/>
+    <mergeCell ref="X22:X23"/>
+    <mergeCell ref="X24:X25"/>
+    <mergeCell ref="X26:X27"/>
+    <mergeCell ref="X28:X29"/>
+    <mergeCell ref="X30:X31"/>
     <mergeCell ref="D62:D63"/>
     <mergeCell ref="X32:X33"/>
     <mergeCell ref="X34:X35"/>
@@ -3098,50 +3130,18 @@
     <mergeCell ref="N40:N41"/>
     <mergeCell ref="S32:S33"/>
     <mergeCell ref="S34:S35"/>
-    <mergeCell ref="S28:S29"/>
-    <mergeCell ref="S30:S31"/>
-    <mergeCell ref="X22:X23"/>
-    <mergeCell ref="X24:X25"/>
-    <mergeCell ref="X26:X27"/>
-    <mergeCell ref="X28:X29"/>
-    <mergeCell ref="X30:X31"/>
-    <mergeCell ref="S36:S37"/>
-    <mergeCell ref="S38:S39"/>
-    <mergeCell ref="N32:N33"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="N24:N25"/>
-    <mergeCell ref="N26:N27"/>
-    <mergeCell ref="N28:N29"/>
-    <mergeCell ref="N30:N31"/>
-    <mergeCell ref="S22:S23"/>
-    <mergeCell ref="S24:S25"/>
-    <mergeCell ref="S26:S27"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="S50:S51"/>
-    <mergeCell ref="S52:S53"/>
-    <mergeCell ref="S54:S55"/>
-    <mergeCell ref="S56:S57"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="I36:I37"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="I40:I41"/>
-    <mergeCell ref="I42:I43"/>
-    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="I60:I61"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="N54:N55"/>
+    <mergeCell ref="N56:N57"/>
+    <mergeCell ref="N58:N59"/>
+    <mergeCell ref="I54:I55"/>
+    <mergeCell ref="I56:I57"/>
+    <mergeCell ref="I58:I59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3152,7 +3152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30648F82-500A-4C87-8FCA-AB2A908FC479}">
   <dimension ref="A1:X58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
@@ -3806,12 +3806,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="N13:N14"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="I15:I16"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="I13:I14"/>
-    <mergeCell ref="N13:N14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
karger 2.0 is done
</commit_message>
<xml_diff>
--- a/excel/karger_burma14.xlsx
+++ b/excel/karger_burma14.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dokumenty\studia\praca_dyplomowa\git_magisterka\magisterka\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7B161C-EEDB-419B-8729-D1EE83C96235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00071A02-7860-4F3E-8FD4-B8AE78BC0D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7A6D875E-0F67-4653-8D10-21F433F1A622}"/>
   </bookViews>
@@ -233,9 +233,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
+      <xdr:colOff>323850</xdr:colOff>
       <xdr:row>89</xdr:row>
-      <xdr:rowOff>173624</xdr:rowOff>
+      <xdr:rowOff>177434</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -619,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB8272D6-92E0-46DF-A61E-1D1AF8F3CB02}">
   <dimension ref="A1:X67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="N85" sqref="N85"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2371,11 +2371,11 @@
         <v>3</v>
       </c>
       <c r="M40">
-        <v>211</v>
+        <v>455</v>
       </c>
       <c r="N40" s="6">
         <f t="shared" ref="N40" si="36">MIN(M40:M41)</f>
-        <v>211</v>
+        <v>247</v>
       </c>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
@@ -3070,6 +3070,62 @@
     </row>
   </sheetData>
   <mergeCells count="72">
+    <mergeCell ref="N54:N55"/>
+    <mergeCell ref="N56:N57"/>
+    <mergeCell ref="N58:N59"/>
+    <mergeCell ref="I54:I55"/>
+    <mergeCell ref="I56:I57"/>
+    <mergeCell ref="I58:I59"/>
+    <mergeCell ref="I60:I61"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="X32:X33"/>
+    <mergeCell ref="X34:X35"/>
+    <mergeCell ref="X36:X37"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="I50:I51"/>
+    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="N50:N51"/>
+    <mergeCell ref="N52:N53"/>
+    <mergeCell ref="N34:N35"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="N38:N39"/>
+    <mergeCell ref="N40:N41"/>
+    <mergeCell ref="S32:S33"/>
+    <mergeCell ref="S34:S35"/>
+    <mergeCell ref="S28:S29"/>
+    <mergeCell ref="S30:S31"/>
+    <mergeCell ref="X22:X23"/>
+    <mergeCell ref="X24:X25"/>
+    <mergeCell ref="X26:X27"/>
+    <mergeCell ref="X28:X29"/>
+    <mergeCell ref="X30:X31"/>
+    <mergeCell ref="S36:S37"/>
+    <mergeCell ref="S38:S39"/>
+    <mergeCell ref="N32:N33"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="N26:N27"/>
+    <mergeCell ref="N28:N29"/>
+    <mergeCell ref="N30:N31"/>
+    <mergeCell ref="S22:S23"/>
+    <mergeCell ref="S24:S25"/>
+    <mergeCell ref="S26:S27"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D30:D31"/>
     <mergeCell ref="D32:D33"/>
     <mergeCell ref="S50:S51"/>
     <mergeCell ref="S52:S53"/>
@@ -3086,62 +3142,6 @@
     <mergeCell ref="I40:I41"/>
     <mergeCell ref="I42:I43"/>
     <mergeCell ref="I32:I33"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="S36:S37"/>
-    <mergeCell ref="S38:S39"/>
-    <mergeCell ref="N32:N33"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="N24:N25"/>
-    <mergeCell ref="N26:N27"/>
-    <mergeCell ref="N28:N29"/>
-    <mergeCell ref="N30:N31"/>
-    <mergeCell ref="S22:S23"/>
-    <mergeCell ref="S24:S25"/>
-    <mergeCell ref="S26:S27"/>
-    <mergeCell ref="S28:S29"/>
-    <mergeCell ref="S30:S31"/>
-    <mergeCell ref="X22:X23"/>
-    <mergeCell ref="X24:X25"/>
-    <mergeCell ref="X26:X27"/>
-    <mergeCell ref="X28:X29"/>
-    <mergeCell ref="X30:X31"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="X32:X33"/>
-    <mergeCell ref="X34:X35"/>
-    <mergeCell ref="X36:X37"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="I50:I51"/>
-    <mergeCell ref="I52:I53"/>
-    <mergeCell ref="N50:N51"/>
-    <mergeCell ref="N52:N53"/>
-    <mergeCell ref="N34:N35"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="N38:N39"/>
-    <mergeCell ref="N40:N41"/>
-    <mergeCell ref="S32:S33"/>
-    <mergeCell ref="S34:S35"/>
-    <mergeCell ref="I60:I61"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="N54:N55"/>
-    <mergeCell ref="N56:N57"/>
-    <mergeCell ref="N58:N59"/>
-    <mergeCell ref="I54:I55"/>
-    <mergeCell ref="I56:I57"/>
-    <mergeCell ref="I58:I59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>